<commit_message>
finishing DNS script generator + developind DHCP feature
</commit_message>
<xml_diff>
--- a/hosts_definition.xlsx
+++ b/hosts_definition.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t xml:space="preserve">hostname</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">mac-address</t>
   </si>
   <si>
+    <t xml:space="preserve">mx-preference</t>
+  </si>
+  <si>
     <t xml:space="preserve">test1</t>
   </si>
   <si>
@@ -53,6 +56,30 @@
   </si>
   <si>
     <t xml:space="preserve">02:03:04:05:06:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int.domain.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email.domain.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.2.5</t>
   </si>
 </sst>
 </file>
@@ -67,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -172,18 +200,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -199,32 +228,74 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>